<commit_message>
updated the submission log
</commit_message>
<xml_diff>
--- a/Kaggle-Competitions/Red-Hat/submission_log.xlsx
+++ b/Kaggle-Competitions/Red-Hat/submission_log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emason\Documents\Other\Kaggle\Red Hat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsullivan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22250" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22245" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>n_estimators=100</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Preprocessing Notes</t>
+  </si>
+  <si>
+    <t>XGB</t>
+  </si>
+  <si>
+    <t>eta = 0.03</t>
+  </si>
+  <si>
+    <t>eta = 0.015</t>
+  </si>
+  <si>
+    <t>eta=0.06</t>
   </si>
 </sst>
 </file>
@@ -424,38 +436,38 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1">
         <f>INDEX(A6:A56,MATCH(B2,B6:B56,0))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
         <f>MAX(B6:B67)</f>
-        <v>0.89899799999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.97869899999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -475,7 +487,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -498,7 +510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -524,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -547,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -567,92 +579,128 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>0.97869899999999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>0.97797199999999995</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>0.97828599999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
updated submission log and fixed issue with preproc_new
</commit_message>
<xml_diff>
--- a/Kaggle-Competitions/Red-Hat/submission_log.xlsx
+++ b/Kaggle-Competitions/Red-Hat/submission_log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emason\Documents\Other\Kaggle\Red Hat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emason\Documents\GitHub\Machine-Learning\Kaggle-Competitions\Red-Hat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22250" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="6940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>n_estimators=100</t>
   </si>
@@ -69,19 +69,79 @@
   </si>
   <si>
     <t>Preprocessing Notes</t>
+  </si>
+  <si>
+    <t>XGB</t>
+  </si>
+  <si>
+    <t>eta = 0.03</t>
+  </si>
+  <si>
+    <t>eta = 0.015</t>
+  </si>
+  <si>
+    <t>eta=0.06</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>n_estimators= 120</t>
+  </si>
+  <si>
+    <t>used pre_proc new with activity type fractions - messed up test sets</t>
+  </si>
+  <si>
+    <r>
+      <t>0.873883</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>used pre_proc new with activity type totals - messed up test sets</t>
+  </si>
+  <si>
+    <t>used pre_proc new with activity type totals - not messed up test sets</t>
+  </si>
+  <si>
+    <t>Interpolation</t>
+  </si>
+  <si>
+    <t>ripped off "group1 and date trick"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,41 +482,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1">
         <f>INDEX(A6:A56,MATCH(B2,B6:B56,0))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
         <f>MAX(B6:B67)</f>
-        <v>0.89899799999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.98702800000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -465,17 +526,17 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -486,19 +547,22 @@
         <v>42230</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -509,22 +573,25 @@
         <v>42230</v>
       </c>
       <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -535,19 +602,22 @@
         <v>42230</v>
       </c>
       <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -558,101 +628,219 @@
         <v>42231</v>
       </c>
       <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>0.97869899999999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>0.97797199999999995</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>0.97828599999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>0.87998500000000002</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42233</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42234</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>0.878135</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42235</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>0.98702800000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42236</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
updated XGB and submission log
</commit_message>
<xml_diff>
--- a/Kaggle-Competitions/Red-Hat/submission_log.xlsx
+++ b/Kaggle-Competitions/Red-Hat/submission_log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsullivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsullivan\Desktop\Machine-Learning\Kaggle-Competitions\Red-Hat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>n_estimators=100</t>
   </si>
@@ -81,6 +81,22 @@
   </si>
   <si>
     <t>eta=0.06</t>
+  </si>
+  <si>
+    <t>eta=.03</t>
+  </si>
+  <si>
+    <t>added date.x.num, date.y.num, date.x.month, date.y.month
+took out char_1 - char_9</t>
+  </si>
+  <si>
+    <t>added date.x.num, date.y.num, date.x.month, date.y.month</t>
+  </si>
+  <si>
+    <t>added group_month feature</t>
+  </si>
+  <si>
+    <t>added group_month_year feature, removed group_month</t>
   </si>
 </sst>
 </file>
@@ -116,9 +132,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +455,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +466,7 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -455,7 +475,7 @@
       </c>
       <c r="B1">
         <f>INDEX(A6:A56,MATCH(B2,B6:B56,0))</f>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -464,7 +484,7 @@
       </c>
       <c r="B2">
         <f>MAX(B6:B67)</f>
-        <v>0.97869899999999999</v>
+        <v>0.98486200000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -630,24 +650,84 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.97889599999999999</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
+      </c>
+      <c r="B14">
+        <v>0.97886200000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42234</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
+      <c r="B15">
+        <v>0.98378100000000002</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42238</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
+      </c>
+      <c r="B16">
+        <v>0.98486200000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42238</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>